<commit_message>
adicionar endpoints para FichaPadrao e ajustar lógica de serialização
</commit_message>
<xml_diff>
--- a/Almoxarifado/template/ficha_epi.xlsx
+++ b/Almoxarifado/template/ficha_epi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tecnika\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tecnika\Documents\Visual Code\TK\api\Almoxarifado\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66582F72-A204-4D48-94D5-5CCC37041D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F940AA7-95CC-4B44-A9B0-5BA5D9248231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3015" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{17386B77-2743-46F1-8E64-F49D792D322D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{17386B77-2743-46F1-8E64-F49D792D322D}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -111,9 +111,6 @@
     <t>___ /___ /____</t>
   </si>
   <si>
-    <t>CPF:</t>
-  </si>
-  <si>
     <t>*Código para devolução do EPI: A - Acidente; D - Danificado; I - Inadequado; T - Tempo de Uso; E - Extraviado; O – Outros</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t xml:space="preserve"> ___ /___ /___ |   </t>
+  </si>
+  <si>
+    <t>RG:</t>
   </si>
 </sst>
 </file>
@@ -756,40 +756,133 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -807,122 +900,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1307,7 +1307,7 @@
   <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="A8" sqref="A8:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1325,140 +1325,140 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46"/>
-      <c r="B1" s="47"/>
-      <c r="C1" s="29" t="s">
+      <c r="A1" s="55"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="31"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="79"/>
       <c r="J1" s="25" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="34"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="82"/>
       <c r="J2" s="26" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
-      <c r="B3" s="49"/>
-      <c r="C3" s="67" t="s">
+      <c r="A3" s="57"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="70"/>
       <c r="J3" s="27" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="50"/>
-      <c r="B4" s="51"/>
-      <c r="C4" s="52" t="s">
+      <c r="A4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="54"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="63"/>
       <c r="J4" s="28">
         <v>42486</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="72"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="44"/>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="79"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="74"/>
-      <c r="J6" s="75"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="49"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="83" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="76"/>
-      <c r="C7" s="76"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="84" t="s">
+      <c r="A7" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="77"/>
-      <c r="G7" s="84" t="s">
+      <c r="F7" s="51"/>
+      <c r="G7" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="77"/>
+      <c r="H7" s="51"/>
       <c r="I7" s="22"/>
       <c r="J7" s="23"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="65"/>
-      <c r="H8" s="65"/>
-      <c r="I8" s="65"/>
-      <c r="J8" s="66"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="39"/>
     </row>
     <row r="9" spans="1:10" s="2" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="62"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="63"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="36"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
@@ -1481,57 +1481,57 @@
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="55" t="s">
+      <c r="A12" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="57" t="s">
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="66" t="s">
         <v>16</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="39" t="s">
+      <c r="G12" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="35" t="s">
+      <c r="H12" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="39" t="s">
+      <c r="I12" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="J12" s="59" t="s">
+      <c r="J12" s="30" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="56"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="58"/>
+      <c r="A13" s="65"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="67"/>
       <c r="F13" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="40"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="60"/>
+        <v>26</v>
+      </c>
+      <c r="G13" s="33"/>
+      <c r="H13" s="84"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="31"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
       <c r="E14" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="82" t="s">
-        <v>28</v>
+      <c r="F14" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="8"/>
@@ -1540,14 +1540,14 @@
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
       <c r="E15" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="82" t="s">
-        <v>28</v>
+      <c r="F15" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G15" s="10"/>
       <c r="H15" s="8"/>
@@ -1556,14 +1556,14 @@
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
       <c r="E16" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="82" t="s">
-        <v>28</v>
+      <c r="F16" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G16" s="10"/>
       <c r="H16" s="8"/>
@@ -1572,14 +1572,14 @@
     </row>
     <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
       <c r="E17" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="82" t="s">
-        <v>28</v>
+      <c r="F17" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G17" s="10"/>
       <c r="H17" s="8"/>
@@ -1588,14 +1588,14 @@
     </row>
     <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
       <c r="E18" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="82" t="s">
-        <v>28</v>
+      <c r="F18" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G18" s="10"/>
       <c r="H18" s="8"/>
@@ -1604,14 +1604,14 @@
     </row>
     <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
       <c r="E19" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="82" t="s">
-        <v>28</v>
+      <c r="F19" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G19" s="10"/>
       <c r="H19" s="8"/>
@@ -1620,14 +1620,14 @@
     </row>
     <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
       <c r="E20" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="82" t="s">
-        <v>28</v>
+      <c r="F20" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G20" s="10"/>
       <c r="H20" s="8"/>
@@ -1636,14 +1636,14 @@
     </row>
     <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
+      <c r="B21" s="54"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
       <c r="E21" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="82" t="s">
-        <v>28</v>
+      <c r="F21" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G21" s="10"/>
       <c r="H21" s="8"/>
@@ -1652,14 +1652,14 @@
     </row>
     <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
       <c r="E22" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="82" t="s">
-        <v>28</v>
+      <c r="F22" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G22" s="10"/>
       <c r="H22" s="8"/>
@@ -1668,14 +1668,14 @@
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
       <c r="E23" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="82" t="s">
-        <v>28</v>
+      <c r="F23" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G23" s="10"/>
       <c r="H23" s="8"/>
@@ -1684,14 +1684,14 @@
     </row>
     <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
       <c r="E24" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="82" t="s">
-        <v>28</v>
+      <c r="F24" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G24" s="10"/>
       <c r="H24" s="8"/>
@@ -1700,14 +1700,14 @@
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
       <c r="E25" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="82" t="s">
-        <v>28</v>
+      <c r="F25" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G25" s="10"/>
       <c r="H25" s="8"/>
@@ -1716,14 +1716,14 @@
     </row>
     <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
       <c r="E26" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="82" t="s">
-        <v>28</v>
+      <c r="F26" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G26" s="10"/>
       <c r="H26" s="8"/>
@@ -1732,14 +1732,14 @@
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
       <c r="E27" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="82" t="s">
-        <v>28</v>
+      <c r="F27" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G27" s="10"/>
       <c r="H27" s="8"/>
@@ -1748,14 +1748,14 @@
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
       <c r="E28" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="82" t="s">
-        <v>28</v>
+      <c r="F28" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="8"/>
@@ -1764,14 +1764,14 @@
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="54"/>
       <c r="E29" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F29" s="82" t="s">
-        <v>28</v>
+      <c r="F29" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G29" s="10"/>
       <c r="H29" s="8"/>
@@ -1780,14 +1780,14 @@
     </row>
     <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
+      <c r="B30" s="54"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="54"/>
       <c r="E30" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F30" s="82" t="s">
-        <v>28</v>
+      <c r="F30" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G30" s="10"/>
       <c r="H30" s="8"/>
@@ -1796,14 +1796,14 @@
     </row>
     <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
+      <c r="B31" s="54"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="54"/>
       <c r="E31" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F31" s="82" t="s">
-        <v>28</v>
+      <c r="F31" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G31" s="10"/>
       <c r="H31" s="8"/>
@@ -1812,14 +1812,14 @@
     </row>
     <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
-      <c r="B32" s="37"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
+      <c r="B32" s="54"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
       <c r="E32" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F32" s="82" t="s">
-        <v>28</v>
+      <c r="F32" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G32" s="10"/>
       <c r="H32" s="8"/>
@@ -1828,14 +1828,14 @@
     </row>
     <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="54"/>
       <c r="E33" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F33" s="82" t="s">
-        <v>28</v>
+      <c r="F33" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G33" s="10"/>
       <c r="H33" s="8"/>
@@ -1844,14 +1844,14 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
-      <c r="B34" s="37"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="37"/>
+      <c r="B34" s="54"/>
+      <c r="C34" s="54"/>
+      <c r="D34" s="54"/>
       <c r="E34" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F34" s="82" t="s">
-        <v>28</v>
+      <c r="F34" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G34" s="10"/>
       <c r="H34" s="8"/>
@@ -1860,14 +1860,14 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
-      <c r="B35" s="37"/>
-      <c r="C35" s="37"/>
-      <c r="D35" s="37"/>
+      <c r="B35" s="54"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="54"/>
       <c r="E35" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F35" s="82" t="s">
-        <v>28</v>
+      <c r="F35" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G35" s="10"/>
       <c r="H35" s="8"/>
@@ -1876,14 +1876,14 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
-      <c r="B36" s="37"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="37"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="54"/>
       <c r="E36" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F36" s="82" t="s">
-        <v>28</v>
+      <c r="F36" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G36" s="10"/>
       <c r="H36" s="8"/>
@@ -1892,14 +1892,14 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="12"/>
-      <c r="B37" s="37"/>
-      <c r="C37" s="37"/>
-      <c r="D37" s="37"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
       <c r="E37" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F37" s="82" t="s">
-        <v>28</v>
+      <c r="F37" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G37" s="10"/>
       <c r="H37" s="8"/>
@@ -1908,14 +1908,14 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="12"/>
-      <c r="B38" s="37"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="37"/>
+      <c r="B38" s="54"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="54"/>
       <c r="E38" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F38" s="82" t="s">
-        <v>28</v>
+      <c r="F38" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G38" s="10"/>
       <c r="H38" s="8"/>
@@ -1924,14 +1924,14 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
-      <c r="B39" s="37"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="37"/>
+      <c r="B39" s="54"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="54"/>
       <c r="E39" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F39" s="82" t="s">
-        <v>28</v>
+      <c r="F39" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G39" s="10"/>
       <c r="H39" s="8"/>
@@ -1940,14 +1940,14 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="37"/>
+      <c r="B40" s="54"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="54"/>
       <c r="E40" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F40" s="82" t="s">
-        <v>28</v>
+      <c r="F40" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G40" s="10"/>
       <c r="H40" s="8"/>
@@ -1956,14 +1956,14 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
-      <c r="B41" s="37"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="37"/>
+      <c r="B41" s="54"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="54"/>
       <c r="E41" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F41" s="82" t="s">
-        <v>28</v>
+      <c r="F41" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G41" s="10"/>
       <c r="H41" s="8"/>
@@ -1972,14 +1972,14 @@
     </row>
     <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="14"/>
-      <c r="B42" s="38"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
+      <c r="B42" s="71"/>
+      <c r="C42" s="71"/>
+      <c r="D42" s="71"/>
       <c r="E42" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F42" s="82" t="s">
-        <v>28</v>
+      <c r="F42" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="G42" s="16"/>
       <c r="H42" s="15"/>
@@ -1987,47 +1987,42 @@
       <c r="J42" s="17"/>
     </row>
     <row r="43" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="41" t="s">
+      <c r="A43" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="B43" s="42"/>
-      <c r="C43" s="42"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="42"/>
-      <c r="F43" s="43" t="s">
+      <c r="B43" s="73"/>
+      <c r="C43" s="73"/>
+      <c r="D43" s="73"/>
+      <c r="E43" s="73"/>
+      <c r="F43" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="G43" s="43"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
-      <c r="J43" s="44"/>
+      <c r="G43" s="74"/>
+      <c r="H43" s="74"/>
+      <c r="I43" s="74"/>
+      <c r="J43" s="75"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="A9:J9"/>
-    <mergeCell ref="A8:J8"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="A1:B4"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B21:D21"/>
     <mergeCell ref="B42:D42"/>
     <mergeCell ref="G12:G13"/>
     <mergeCell ref="A43:E43"/>
@@ -2044,22 +2039,27 @@
     <mergeCell ref="B12:D13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="A1:B4"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="C3:I3"/>
     <mergeCell ref="C1:I2"/>
     <mergeCell ref="H12:H13"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="A8:J8"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A7:D7"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>